<commit_message>
Fixing by 1 off error in CreateOutput method.
</commit_message>
<xml_diff>
--- a/abstract_doi_finder/input/inputtest.xlsx
+++ b/abstract_doi_finder/input/inputtest.xlsx
@@ -439,9 +439,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.66"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="22.26" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="20.13" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="10.66" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="2" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,106 +890,106 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="11.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="12.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="12.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="13.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="40" style="1" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="47" style="1" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="14.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="13.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="57" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="14.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="7.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="8.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="1" width="7.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="1" width="13.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="74" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="1" width="11.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="82" style="1" width="11.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="1" width="8.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="1" width="12.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="1" width="12.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="1" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="1" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="1" width="12.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="1" width="10.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="1" width="11.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="1" width="10.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="1" width="11.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="109" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="111" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="1" width="12.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="1" width="11.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="116" style="1" width="12.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="123" style="1" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="124" style="1" width="11.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="125" style="3" width="9"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="27.61" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="7.16" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="7.4" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="6.73" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.0" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="12.73" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="9.86" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.26" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="12" customWidth="true" hidden="false" style="1" width="9.86" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="10.13" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="16" customWidth="true" hidden="false" style="1" width="10.85" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="11.26" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="9.86" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="11.73" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="10.13" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="22" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="11.58" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="24" customWidth="true" hidden="false" style="1" width="11.12" collapsed="true" outlineLevel="0"/>
+    <col min="25" max="25" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="10.85" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="8.73" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="11.12" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="30" customWidth="true" hidden="false" style="1" width="10.0" collapsed="true" outlineLevel="0"/>
+    <col min="31" max="31" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="13.15" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="34" customWidth="true" hidden="false" style="1" width="12.15" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="12.26" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="36" customWidth="true" hidden="false" style="1" width="12.61" collapsed="true" outlineLevel="0"/>
+    <col min="37" max="37" customWidth="true" hidden="false" style="1" width="12.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="12.88" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="13.73" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="42" customWidth="true" hidden="false" style="1" width="10.26" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="10.13" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="12.61" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="48" customWidth="true" hidden="false" style="1" width="12.61" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="51" customWidth="true" hidden="false" style="1" width="13.87" collapsed="true" outlineLevel="0"/>
+    <col min="52" max="52" customWidth="true" hidden="false" style="1" width="13.6" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="12.88" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="1" width="14.26" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="55" customWidth="true" hidden="false" style="1" width="13.26" collapsed="true" outlineLevel="0"/>
+    <col min="56" max="56" customWidth="true" hidden="false" style="1" width="13.73" collapsed="true" outlineLevel="0"/>
+    <col min="57" max="58" customWidth="true" hidden="false" style="1" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="59" max="59" customWidth="true" hidden="false" style="1" width="13.6" collapsed="true" outlineLevel="0"/>
+    <col min="60" max="60" customWidth="true" hidden="false" style="1" width="11.85" collapsed="true" outlineLevel="0"/>
+    <col min="61" max="61" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="62" max="62" customWidth="true" hidden="false" style="1" width="12.88" collapsed="true" outlineLevel="0"/>
+    <col min="63" max="63" customWidth="true" hidden="false" style="1" width="14.26" collapsed="true" outlineLevel="0"/>
+    <col min="64" max="64" customWidth="true" hidden="false" style="1" width="7.16" collapsed="true" outlineLevel="0"/>
+    <col min="65" max="65" customWidth="true" hidden="false" style="1" width="7.4" collapsed="true" outlineLevel="0"/>
+    <col min="66" max="66" customWidth="true" hidden="false" style="1" width="6.85" collapsed="true" outlineLevel="0"/>
+    <col min="67" max="67" customWidth="true" hidden="false" style="1" width="8.26" collapsed="true" outlineLevel="0"/>
+    <col min="69" max="69" customWidth="true" hidden="false" style="1" width="9.6" collapsed="true" outlineLevel="0"/>
+    <col min="70" max="70" customWidth="true" hidden="false" style="1" width="11.0" collapsed="true" outlineLevel="0"/>
+    <col min="71" max="71" customWidth="true" hidden="false" style="1" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="72" max="72" customWidth="true" hidden="false" style="1" width="7.73" collapsed="true" outlineLevel="0"/>
+    <col min="73" max="73" customWidth="true" hidden="false" style="1" width="13.73" collapsed="true" outlineLevel="0"/>
+    <col min="74" max="75" customWidth="true" hidden="false" style="1" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="76" max="76" customWidth="true" hidden="false" style="1" width="11.58" collapsed="true" outlineLevel="0"/>
+    <col min="77" max="77" customWidth="true" hidden="false" style="1" width="11.73" collapsed="true" outlineLevel="0"/>
+    <col min="78" max="78" customWidth="true" hidden="false" style="1" width="11.39" collapsed="true" outlineLevel="0"/>
+    <col min="79" max="79" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="80" max="80" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
+    <col min="82" max="83" customWidth="true" hidden="false" style="1" width="11.73" collapsed="true" outlineLevel="0"/>
+    <col min="84" max="84" customWidth="true" hidden="false" style="1" width="11.12" collapsed="true" outlineLevel="0"/>
+    <col min="85" max="85" customWidth="true" hidden="false" style="1" width="11.39" collapsed="true" outlineLevel="0"/>
+    <col min="86" max="86" customWidth="true" hidden="false" style="1" width="8.87" collapsed="true" outlineLevel="0"/>
+    <col min="87" max="87" customWidth="true" hidden="false" style="1" width="12.73" collapsed="true" outlineLevel="0"/>
+    <col min="88" max="88" customWidth="true" hidden="false" style="1" width="11.39" collapsed="true" outlineLevel="0"/>
+    <col min="89" max="89" customWidth="true" hidden="false" style="1" width="11.58" collapsed="true" outlineLevel="0"/>
+    <col min="90" max="90" customWidth="true" hidden="false" style="1" width="11.12" collapsed="true" outlineLevel="0"/>
+    <col min="91" max="91" customWidth="true" hidden="false" style="1" width="12.4" collapsed="true" outlineLevel="0"/>
+    <col min="92" max="92" customWidth="true" hidden="false" style="1" width="12.61" collapsed="true" outlineLevel="0"/>
+    <col min="93" max="93" customWidth="true" hidden="false" style="1" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="94" max="94" customWidth="true" hidden="false" style="1" width="11.39" collapsed="true" outlineLevel="0"/>
+    <col min="95" max="95" customWidth="true" hidden="false" style="1" width="12.88" collapsed="true" outlineLevel="0"/>
+    <col min="96" max="96" customWidth="true" hidden="false" style="1" width="11.85" collapsed="true" outlineLevel="0"/>
+    <col min="97" max="97" customWidth="true" hidden="false" style="1" width="12.88" collapsed="true" outlineLevel="0"/>
+    <col min="98" max="98" customWidth="true" hidden="false" style="1" width="13.4" collapsed="true" outlineLevel="0"/>
+    <col min="99" max="99" customWidth="true" hidden="false" style="1" width="12.88" collapsed="true" outlineLevel="0"/>
+    <col min="100" max="100" customWidth="true" hidden="false" style="1" width="12.15" collapsed="true" outlineLevel="0"/>
+    <col min="101" max="101" customWidth="true" hidden="false" style="1" width="12.61" collapsed="true" outlineLevel="0"/>
+    <col min="102" max="102" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="103" max="103" customWidth="true" hidden="false" style="1" width="11.12" collapsed="true" outlineLevel="0"/>
+    <col min="104" max="104" customWidth="true" hidden="false" style="1" width="10.4" collapsed="true" outlineLevel="0"/>
+    <col min="105" max="105" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
+    <col min="106" max="106" customWidth="true" hidden="false" style="1" width="11.26" collapsed="true" outlineLevel="0"/>
+    <col min="107" max="107" customWidth="true" hidden="false" style="1" width="10.59" collapsed="true" outlineLevel="0"/>
+    <col min="108" max="108" customWidth="true" hidden="false" style="1" width="11.73" collapsed="true" outlineLevel="0"/>
+    <col min="109" max="109" customWidth="true" hidden="false" style="1" width="11.85" collapsed="true" outlineLevel="0"/>
+    <col min="110" max="110" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
+    <col min="111" max="113" customWidth="true" hidden="false" style="1" width="12.0" collapsed="true" outlineLevel="0"/>
+    <col min="114" max="114" customWidth="true" hidden="false" style="1" width="12.4" collapsed="true" outlineLevel="0"/>
+    <col min="115" max="115" customWidth="true" hidden="false" style="1" width="11.73" collapsed="true" outlineLevel="0"/>
+    <col min="116" max="122" customWidth="true" hidden="false" style="1" width="12.26" collapsed="true" outlineLevel="0"/>
+    <col min="123" max="123" customWidth="true" hidden="false" style="1" width="13.15" collapsed="true" outlineLevel="0"/>
+    <col min="124" max="124" customWidth="true" hidden="false" style="1" width="11.73" collapsed="true" outlineLevel="0"/>
+    <col min="125" max="16384" customWidth="false" hidden="false" style="3" width="9.0" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6057,7 +6057,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
+    <col min="16383" max="16384" customWidth="true" hidden="false" style="1" width="11.53" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="128.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>